<commit_message>
fixing automatic mapping of country codes and csv column names in the new PECD processor
</commit_message>
<xml_diff>
--- a/src_files/data_files/unittypedata_maf2020.xlsx
+++ b/src_files/data_files/unittypedata_maf2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60ED63F8-C02F-47E5-8069-C7065017D442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD50CD52-3A50-4BAA-BE14-8A8A424C2B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1232,10 +1232,10 @@
   <dimension ref="A1:AJ93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="W18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ25" sqref="AJ25"/>
+      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixing fuels of multiple biomass retrofitted units
</commit_message>
<xml_diff>
--- a/src_files/data_files/unittypedata_maf2020.xlsx
+++ b/src_files/data_files/unittypedata_maf2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\NEBB-alt\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6EA627-E830-4095-86EF-6369DE239074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EE439F-6967-4F92-9563-DAFA8192602E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unittypedata" sheetId="1" r:id="rId1"/>
@@ -1214,10 +1214,10 @@
   <dimension ref="A1:AO89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="Y53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG73" sqref="AG73"/>
+      <selection pane="bottomRight" activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4151,8 +4151,8 @@
       <c r="I37" t="s">
         <v>234</v>
       </c>
-      <c r="J37" t="s">
-        <v>19</v>
+      <c r="J37" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="K37" t="s">
         <v>71</v>
@@ -4332,7 +4332,7 @@
         <v>234</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="K39" t="s">
         <v>71</v>
@@ -4512,7 +4512,7 @@
         <v>234</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="K41" t="s">
         <v>71</v>
@@ -5234,76 +5234,93 @@
       <c r="B50" s="11">
         <v>1</v>
       </c>
-      <c r="C50" s="7" t="s">
-        <v>104</v>
+      <c r="C50" s="4" t="s">
+        <v>241</v>
       </c>
       <c r="D50" t="s">
-        <v>215</v>
-      </c>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="K50" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="P50" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="Q50" s="7">
-        <v>0</v>
+        <v>243</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" t="s">
+        <v>234</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" t="s">
+        <v>71</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="P50" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>0.4</v>
       </c>
       <c r="R50">
         <v>1</v>
       </c>
-      <c r="S50" s="7">
-        <v>1</v>
-      </c>
-      <c r="T50" s="7"/>
-      <c r="U50" s="7"/>
-      <c r="V50" s="7"/>
-      <c r="W50" s="7"/>
-      <c r="X50" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y50" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z50" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA50" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB50" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC50" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD50" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE50" s="7"/>
-      <c r="AF50" s="7"/>
-      <c r="AG50" s="7"/>
-      <c r="AH50" s="7"/>
-      <c r="AI50" s="7"/>
-      <c r="AJ50" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK50" s="7"/>
-      <c r="AL50" s="7"/>
+      <c r="S50" s="4">
+        <v>2</v>
+      </c>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4">
+        <v>3</v>
+      </c>
+      <c r="V50" s="4">
+        <v>3</v>
+      </c>
+      <c r="W50" s="4">
+        <v>1.94</v>
+      </c>
+      <c r="X50" s="4">
+        <v>70</v>
+      </c>
+      <c r="Y50" s="4">
+        <v>1.94</v>
+      </c>
+      <c r="Z50" s="4">
+        <v>150</v>
+      </c>
+      <c r="AA50" s="4">
+        <v>1.94</v>
+      </c>
+      <c r="AB50" s="4">
+        <v>40</v>
+      </c>
+      <c r="AC50" s="4">
+        <v>12</v>
+      </c>
+      <c r="AD50" s="4">
+        <v>24</v>
+      </c>
+      <c r="AE50" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="AF50" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="AG50" s="4"/>
+      <c r="AH50" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AI50" s="4">
+        <v>-0.16666666666666699</v>
+      </c>
+      <c r="AJ50" s="4">
+        <v>95</v>
+      </c>
+      <c r="AL50" s="2"/>
     </row>
     <row r="51" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
@@ -5312,78 +5329,90 @@
       <c r="B51" s="11">
         <v>1</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>105</v>
+      <c r="C51" s="4" t="s">
+        <v>242</v>
       </c>
       <c r="D51" t="s">
-        <v>214</v>
-      </c>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="K51" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="P51" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="Q51" s="7">
-        <v>0</v>
+        <v>244</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K51" t="s">
+        <v>71</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="P51" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>0.4</v>
       </c>
       <c r="R51">
         <v>1</v>
       </c>
-      <c r="S51" s="7">
-        <v>1</v>
-      </c>
-      <c r="T51" s="7"/>
-      <c r="U51" s="7"/>
-      <c r="V51" s="7"/>
-      <c r="W51" s="7"/>
-      <c r="X51" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y51" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z51" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA51" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB51" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC51" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD51" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE51" s="7"/>
-      <c r="AF51" s="7"/>
-      <c r="AG51" s="7"/>
-      <c r="AH51" s="7"/>
-      <c r="AI51" s="7"/>
-      <c r="AJ51" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK51" s="7">
-        <v>100</v>
-      </c>
-      <c r="AL51" s="7"/>
+      <c r="S51" s="4">
+        <v>2</v>
+      </c>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4">
+        <v>3</v>
+      </c>
+      <c r="V51" s="4">
+        <v>3</v>
+      </c>
+      <c r="W51" s="4">
+        <v>1.94</v>
+      </c>
+      <c r="X51" s="4">
+        <v>70</v>
+      </c>
+      <c r="Y51" s="4">
+        <v>1.94</v>
+      </c>
+      <c r="Z51" s="4">
+        <v>150</v>
+      </c>
+      <c r="AA51" s="4">
+        <v>1.94</v>
+      </c>
+      <c r="AB51" s="4">
+        <v>40</v>
+      </c>
+      <c r="AC51" s="4">
+        <v>12</v>
+      </c>
+      <c r="AD51" s="4">
+        <v>24</v>
+      </c>
+      <c r="AE51" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="AF51" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="AG51" s="4"/>
+      <c r="AH51" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AI51" s="4">
+        <v>-0.16666666666666699</v>
+      </c>
+      <c r="AJ51" s="4">
+        <v>85</v>
+      </c>
     </row>
     <row r="52" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
@@ -5392,75 +5421,76 @@
       <c r="B52" s="11">
         <v>1</v>
       </c>
-      <c r="C52" t="s">
-        <v>45</v>
+      <c r="C52" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="D52" t="s">
-        <v>165</v>
-      </c>
-      <c r="I52" t="s">
-        <v>234</v>
-      </c>
-      <c r="J52" t="s">
-        <v>45</v>
-      </c>
-      <c r="K52" t="s">
-        <v>71</v>
-      </c>
-      <c r="O52">
-        <v>0.35</v>
-      </c>
-      <c r="P52">
-        <v>0.35</v>
-      </c>
-      <c r="Q52">
-        <v>0.5</v>
+        <v>215</v>
+      </c>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="K52" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="P52" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="Q52" s="7">
+        <v>0</v>
       </c>
       <c r="R52">
         <v>1</v>
       </c>
-      <c r="S52">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U52">
-        <v>1</v>
-      </c>
-      <c r="V52">
-        <v>1</v>
-      </c>
-      <c r="W52">
-        <v>0.06</v>
-      </c>
-      <c r="X52">
-        <v>36</v>
-      </c>
-      <c r="Y52">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Z52">
-        <v>38.4</v>
-      </c>
-      <c r="AA52">
-        <v>0.06</v>
-      </c>
-      <c r="AB52">
-        <v>24</v>
-      </c>
-      <c r="AC52">
-        <v>2</v>
-      </c>
-      <c r="AD52">
-        <v>3</v>
-      </c>
-      <c r="AE52">
-        <v>0.08</v>
-      </c>
-      <c r="AF52">
-        <v>0.08</v>
-      </c>
-      <c r="AJ52">
-        <v>38.4</v>
-      </c>
+      <c r="S52" s="7">
+        <v>1</v>
+      </c>
+      <c r="T52" s="7"/>
+      <c r="U52" s="7"/>
+      <c r="V52" s="7"/>
+      <c r="W52" s="7"/>
+      <c r="X52" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y52" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA52" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC52" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD52" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE52" s="7"/>
+      <c r="AF52" s="7"/>
+      <c r="AG52" s="7"/>
+      <c r="AH52" s="7"/>
+      <c r="AI52" s="7"/>
+      <c r="AJ52" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK52" s="7"/>
+      <c r="AL52" s="7"/>
     </row>
     <row r="53" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
@@ -5469,72 +5499,78 @@
       <c r="B53" s="11">
         <v>1</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>31</v>
+      <c r="C53" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="D53" t="s">
-        <v>138</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K53" t="s">
-        <v>71</v>
-      </c>
-      <c r="O53" s="2">
-        <v>0.38</v>
-      </c>
-      <c r="P53" s="2">
-        <v>0.38</v>
-      </c>
-      <c r="Q53" s="2">
-        <v>0.5</v>
+        <v>214</v>
+      </c>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="P53" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="Q53" s="7">
+        <v>0</v>
       </c>
       <c r="R53">
         <v>1</v>
       </c>
-      <c r="S53" s="2">
-        <v>6.6</v>
-      </c>
-      <c r="U53" s="2">
-        <v>10</v>
-      </c>
-      <c r="V53" s="2">
-        <v>10</v>
-      </c>
-      <c r="W53" s="2">
-        <v>5</v>
-      </c>
-      <c r="X53" s="2">
-        <v>50.12</v>
-      </c>
-      <c r="Y53" s="2">
-        <v>5.83</v>
-      </c>
-      <c r="Z53" s="2">
-        <v>81.44</v>
-      </c>
-      <c r="AA53" s="2">
-        <v>2.92</v>
-      </c>
-      <c r="AB53" s="2">
-        <v>42.29</v>
-      </c>
-      <c r="AC53" s="2">
-        <v>12</v>
-      </c>
-      <c r="AD53" s="2">
-        <v>72</v>
-      </c>
-      <c r="AE53" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="AF53" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="AJ53" s="2">
-        <v>81.44</v>
-      </c>
+      <c r="S53" s="7">
+        <v>1</v>
+      </c>
+      <c r="T53" s="7"/>
+      <c r="U53" s="7"/>
+      <c r="V53" s="7"/>
+      <c r="W53" s="7"/>
+      <c r="X53" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y53" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE53" s="7"/>
+      <c r="AF53" s="7"/>
+      <c r="AG53" s="7"/>
+      <c r="AH53" s="7"/>
+      <c r="AI53" s="7"/>
+      <c r="AJ53" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK53" s="7">
+        <v>100</v>
+      </c>
+      <c r="AL53" s="7"/>
     </row>
     <row r="54" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
@@ -5543,88 +5579,88 @@
       <c r="B54" s="11">
         <v>1</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>30</v>
+      <c r="C54" t="s">
+        <v>45</v>
       </c>
       <c r="D54" t="s">
-        <v>142</v>
-      </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
+        <v>165</v>
+      </c>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
       <c r="I54" t="s">
         <v>234</v>
       </c>
-      <c r="J54" s="2" t="s">
-        <v>27</v>
+      <c r="J54" t="s">
+        <v>45</v>
       </c>
       <c r="K54" t="s">
         <v>71</v>
       </c>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2">
-        <v>0.46</v>
-      </c>
-      <c r="P54" s="2">
-        <v>0.46</v>
-      </c>
-      <c r="Q54" s="2">
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54">
+        <v>0.35</v>
+      </c>
+      <c r="P54">
+        <v>0.35</v>
+      </c>
+      <c r="Q54">
         <v>0.5</v>
       </c>
       <c r="R54">
         <v>1</v>
       </c>
-      <c r="S54" s="2">
-        <v>3.3</v>
-      </c>
-      <c r="T54" s="2"/>
-      <c r="U54" s="2">
-        <v>8</v>
-      </c>
-      <c r="V54" s="2">
-        <v>8</v>
-      </c>
-      <c r="W54" s="2">
-        <v>5</v>
-      </c>
-      <c r="X54" s="2">
-        <v>42.29</v>
-      </c>
-      <c r="Y54" s="2">
-        <v>5.83</v>
-      </c>
-      <c r="Z54" s="2">
-        <v>57.17</v>
-      </c>
-      <c r="AA54" s="2">
-        <v>2.92</v>
-      </c>
-      <c r="AB54" s="2">
-        <v>30.54</v>
-      </c>
-      <c r="AC54" s="2">
-        <v>12</v>
-      </c>
-      <c r="AD54" s="2">
-        <v>72</v>
-      </c>
-      <c r="AE54" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="AF54" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="AG54" s="2"/>
-      <c r="AH54" s="2"/>
-      <c r="AI54" s="2"/>
-      <c r="AJ54" s="2">
-        <v>57.17</v>
-      </c>
-      <c r="AK54" s="2"/>
-      <c r="AL54" s="2"/>
+      <c r="S54">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T54"/>
+      <c r="U54">
+        <v>1</v>
+      </c>
+      <c r="V54">
+        <v>1</v>
+      </c>
+      <c r="W54">
+        <v>0.06</v>
+      </c>
+      <c r="X54">
+        <v>36</v>
+      </c>
+      <c r="Y54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z54">
+        <v>38.4</v>
+      </c>
+      <c r="AA54">
+        <v>0.06</v>
+      </c>
+      <c r="AB54">
+        <v>24</v>
+      </c>
+      <c r="AC54">
+        <v>2</v>
+      </c>
+      <c r="AD54">
+        <v>3</v>
+      </c>
+      <c r="AE54">
+        <v>0.08</v>
+      </c>
+      <c r="AF54">
+        <v>0.08</v>
+      </c>
+      <c r="AG54"/>
+      <c r="AH54"/>
+      <c r="AI54"/>
+      <c r="AJ54">
+        <v>38.4</v>
+      </c>
+      <c r="AK54"/>
+      <c r="AL54"/>
     </row>
     <row r="55" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
@@ -5633,88 +5669,72 @@
       <c r="B55" s="11">
         <v>1</v>
       </c>
-      <c r="C55" t="s">
-        <v>28</v>
+      <c r="C55" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>140</v>
-      </c>
-      <c r="E55"/>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55" t="s">
-        <v>234</v>
-      </c>
-      <c r="J55" t="s">
+        <v>138</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K55" t="s">
         <v>71</v>
       </c>
-      <c r="L55"/>
-      <c r="M55"/>
-      <c r="N55"/>
-      <c r="O55">
-        <v>0.35</v>
-      </c>
-      <c r="P55">
-        <v>0.35</v>
-      </c>
-      <c r="Q55">
+      <c r="O55" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="P55" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="Q55" s="2">
         <v>0.5</v>
       </c>
       <c r="R55">
         <v>1</v>
       </c>
-      <c r="S55">
-        <v>3.3</v>
-      </c>
-      <c r="T55"/>
-      <c r="U55">
-        <v>11</v>
-      </c>
-      <c r="V55">
-        <v>11</v>
-      </c>
-      <c r="W55">
+      <c r="S55" s="2">
+        <v>6.6</v>
+      </c>
+      <c r="U55" s="2">
+        <v>10</v>
+      </c>
+      <c r="V55" s="2">
+        <v>10</v>
+      </c>
+      <c r="W55" s="2">
         <v>5</v>
       </c>
-      <c r="X55">
-        <v>69.69</v>
-      </c>
-      <c r="Y55">
+      <c r="X55" s="2">
+        <v>50.12</v>
+      </c>
+      <c r="Y55" s="2">
         <v>5.83</v>
       </c>
-      <c r="Z55">
-        <v>93.97</v>
-      </c>
-      <c r="AA55">
+      <c r="Z55" s="2">
+        <v>81.44</v>
+      </c>
+      <c r="AA55" s="2">
         <v>2.92</v>
       </c>
-      <c r="AB55">
-        <v>49.33</v>
-      </c>
-      <c r="AC55">
+      <c r="AB55" s="2">
+        <v>42.29</v>
+      </c>
+      <c r="AC55" s="2">
         <v>12</v>
       </c>
-      <c r="AD55">
+      <c r="AD55" s="2">
         <v>72</v>
       </c>
-      <c r="AE55">
+      <c r="AE55" s="2">
         <v>0.02</v>
       </c>
-      <c r="AF55">
+      <c r="AF55" s="2">
         <v>0.05</v>
       </c>
-      <c r="AG55"/>
-      <c r="AH55"/>
-      <c r="AI55"/>
-      <c r="AJ55">
-        <v>93.97</v>
-      </c>
-      <c r="AK55"/>
-      <c r="AL55"/>
+      <c r="AJ55" s="2">
+        <v>81.44</v>
+      </c>
     </row>
     <row r="56" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
@@ -5724,18 +5744,20 @@
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
-      <c r="I56" s="19"/>
+      <c r="I56" t="s">
+        <v>234</v>
+      </c>
       <c r="J56" s="2" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="K56" t="s">
         <v>71</v>
@@ -5744,10 +5766,10 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2">
-        <v>0.35</v>
+        <v>0.46</v>
       </c>
       <c r="P56" s="2">
-        <v>0.35</v>
+        <v>0.46</v>
       </c>
       <c r="Q56" s="2">
         <v>0.5</v>
@@ -5760,28 +5782,28 @@
       </c>
       <c r="T56" s="2"/>
       <c r="U56" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="V56" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="W56" s="2">
         <v>5</v>
       </c>
       <c r="X56" s="2">
-        <v>69.69</v>
+        <v>42.29</v>
       </c>
       <c r="Y56" s="2">
         <v>5.83</v>
       </c>
       <c r="Z56" s="2">
-        <v>93.97</v>
+        <v>57.17</v>
       </c>
       <c r="AA56" s="2">
         <v>2.92</v>
       </c>
       <c r="AB56" s="2">
-        <v>49.33</v>
+        <v>30.54</v>
       </c>
       <c r="AC56" s="2">
         <v>12</v>
@@ -5799,7 +5821,7 @@
       <c r="AH56" s="2"/>
       <c r="AI56" s="2"/>
       <c r="AJ56" s="2">
-        <v>93.97</v>
+        <v>57.17</v>
       </c>
       <c r="AK56" s="2"/>
       <c r="AL56" s="2"/>
@@ -5812,10 +5834,10 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I57" t="s">
         <v>234</v>
@@ -5827,10 +5849,10 @@
         <v>71</v>
       </c>
       <c r="O57">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="P57">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="Q57">
         <v>0.5</v>
@@ -5842,28 +5864,28 @@
         <v>3.3</v>
       </c>
       <c r="U57">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="V57">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="W57">
         <v>5</v>
       </c>
       <c r="X57">
-        <v>50.12</v>
+        <v>69.69</v>
       </c>
       <c r="Y57">
         <v>5.83</v>
       </c>
       <c r="Z57">
-        <v>81.44</v>
+        <v>93.97</v>
       </c>
       <c r="AA57">
         <v>2.92</v>
       </c>
       <c r="AB57">
-        <v>42.29</v>
+        <v>49.33</v>
       </c>
       <c r="AC57">
         <v>12</v>
@@ -5878,7 +5900,7 @@
         <v>0.05</v>
       </c>
       <c r="AJ57">
-        <v>81.44</v>
+        <v>93.97</v>
       </c>
     </row>
     <row r="58" spans="1:38" x14ac:dyDescent="0.25">
@@ -5889,10 +5911,10 @@
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -5909,10 +5931,10 @@
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="P58" s="2">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="Q58" s="2">
         <v>0.5</v>
@@ -5925,28 +5947,28 @@
       </c>
       <c r="T58" s="2"/>
       <c r="U58" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="V58" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="W58" s="2">
         <v>5</v>
       </c>
       <c r="X58" s="2">
-        <v>50.12</v>
+        <v>69.69</v>
       </c>
       <c r="Y58" s="2">
         <v>5.83</v>
       </c>
       <c r="Z58" s="2">
-        <v>81.44</v>
+        <v>93.97</v>
       </c>
       <c r="AA58" s="2">
         <v>2.92</v>
       </c>
       <c r="AB58" s="2">
-        <v>42.29</v>
+        <v>49.33</v>
       </c>
       <c r="AC58" s="2">
         <v>12</v>
@@ -5964,7 +5986,7 @@
       <c r="AH58" s="2"/>
       <c r="AI58" s="2"/>
       <c r="AJ58" s="2">
-        <v>81.44</v>
+        <v>93.97</v>
       </c>
       <c r="AK58" s="2"/>
       <c r="AL58" s="2"/>
@@ -5976,58 +5998,88 @@
       <c r="B59" s="11">
         <v>1</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>113</v>
+      <c r="C59" t="s">
+        <v>29</v>
       </c>
       <c r="D59" t="s">
-        <v>195</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="O59" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="P59" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="Q59" s="4">
-        <v>0</v>
+        <v>141</v>
+      </c>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59" t="s">
+        <v>234</v>
+      </c>
+      <c r="J59" t="s">
+        <v>27</v>
+      </c>
+      <c r="K59" t="s">
+        <v>71</v>
+      </c>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59">
+        <v>0.4</v>
+      </c>
+      <c r="P59">
+        <v>0.4</v>
+      </c>
+      <c r="Q59">
+        <v>0.5</v>
       </c>
       <c r="R59">
         <v>1</v>
       </c>
-      <c r="S59" s="4">
-        <v>1</v>
-      </c>
-      <c r="X59" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y59" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z59" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA59" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB59" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC59" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD59" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ59" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK59" s="5"/>
+      <c r="S59">
+        <v>3.3</v>
+      </c>
+      <c r="T59"/>
+      <c r="U59">
+        <v>9</v>
+      </c>
+      <c r="V59">
+        <v>9</v>
+      </c>
+      <c r="W59">
+        <v>5</v>
+      </c>
+      <c r="X59">
+        <v>50.12</v>
+      </c>
+      <c r="Y59">
+        <v>5.83</v>
+      </c>
+      <c r="Z59">
+        <v>81.44</v>
+      </c>
+      <c r="AA59">
+        <v>2.92</v>
+      </c>
+      <c r="AB59">
+        <v>42.29</v>
+      </c>
+      <c r="AC59">
+        <v>12</v>
+      </c>
+      <c r="AD59">
+        <v>72</v>
+      </c>
+      <c r="AE59">
+        <v>0.02</v>
+      </c>
+      <c r="AF59">
+        <v>0.05</v>
+      </c>
+      <c r="AG59"/>
+      <c r="AH59"/>
+      <c r="AI59"/>
+      <c r="AJ59">
+        <v>81.44</v>
+      </c>
+      <c r="AK59"/>
+      <c r="AL59"/>
     </row>
     <row r="60" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
@@ -6036,60 +6088,86 @@
       <c r="B60" s="11">
         <v>1</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>114</v>
+      <c r="C60" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D60" t="s">
-        <v>196</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="O60" s="4">
-        <v>1</v>
-      </c>
-      <c r="P60" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q60" s="4">
-        <v>0</v>
+        <v>144</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K60" t="s">
+        <v>71</v>
+      </c>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="P60" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="Q60" s="2">
+        <v>0.5</v>
       </c>
       <c r="R60">
         <v>1</v>
       </c>
-      <c r="S60" s="4">
-        <v>0</v>
-      </c>
-      <c r="X60" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA60" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB60" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC60" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD60" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ60" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK60" s="5">
-        <v>924</v>
-      </c>
+      <c r="S60" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="T60" s="2"/>
+      <c r="U60" s="2">
+        <v>9</v>
+      </c>
+      <c r="V60" s="2">
+        <v>9</v>
+      </c>
+      <c r="W60" s="2">
+        <v>5</v>
+      </c>
+      <c r="X60" s="2">
+        <v>50.12</v>
+      </c>
+      <c r="Y60" s="2">
+        <v>5.83</v>
+      </c>
+      <c r="Z60" s="2">
+        <v>81.44</v>
+      </c>
+      <c r="AA60" s="2">
+        <v>2.92</v>
+      </c>
+      <c r="AB60" s="2">
+        <v>42.29</v>
+      </c>
+      <c r="AC60" s="2">
+        <v>12</v>
+      </c>
+      <c r="AD60" s="2">
+        <v>72</v>
+      </c>
+      <c r="AE60" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="AF60" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AG60" s="2"/>
+      <c r="AH60" s="2"/>
+      <c r="AI60" s="2"/>
+      <c r="AJ60" s="2">
+        <v>81.44</v>
+      </c>
+      <c r="AK60" s="2"/>
+      <c r="AL60" s="2"/>
     </row>
     <row r="61" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
@@ -6098,60 +6176,76 @@
       <c r="B61" s="11">
         <v>1</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>89</v>
+      <c r="C61" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="D61" t="s">
-        <v>204</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K61" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O61" s="2">
-        <v>1</v>
-      </c>
-      <c r="P61" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q61" s="2">
+        <v>195</v>
+      </c>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="P61" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="Q61" s="4">
         <v>0</v>
       </c>
       <c r="R61">
         <v>1</v>
       </c>
-      <c r="S61" s="2">
-        <v>0</v>
-      </c>
-      <c r="X61" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y61" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA61" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB61" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC61" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD61" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ61" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK61" s="2">
-        <v>4</v>
-      </c>
+      <c r="S61" s="4">
+        <v>1</v>
+      </c>
+      <c r="T61" s="4"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+      <c r="W61" s="4"/>
+      <c r="X61" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y61" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA61" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB61" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC61" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD61" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE61" s="4"/>
+      <c r="AF61" s="4"/>
+      <c r="AG61" s="4"/>
+      <c r="AH61" s="4"/>
+      <c r="AI61" s="4"/>
+      <c r="AJ61" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK61" s="5"/>
+      <c r="AL61" s="4"/>
     </row>
     <row r="62" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
@@ -6160,78 +6254,60 @@
       <c r="B62" s="11">
         <v>1</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>91</v>
+      <c r="C62" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="D62" t="s">
-        <v>205</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K62" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2">
-        <v>1</v>
-      </c>
-      <c r="P62" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q62" s="2">
+        <v>196</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O62" s="4">
+        <v>1</v>
+      </c>
+      <c r="P62" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="4">
         <v>0</v>
       </c>
       <c r="R62">
         <v>1</v>
       </c>
-      <c r="S62" s="2">
-        <v>30</v>
-      </c>
-      <c r="T62" s="2"/>
-      <c r="U62" s="2"/>
-      <c r="V62" s="2"/>
-      <c r="W62" s="2"/>
-      <c r="X62" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y62" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA62" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB62" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC62" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD62" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE62" s="2"/>
-      <c r="AF62" s="2"/>
-      <c r="AG62" s="2"/>
-      <c r="AH62" s="2"/>
-      <c r="AI62" s="2"/>
-      <c r="AJ62" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK62" s="2">
-        <v>4</v>
-      </c>
-      <c r="AL62" s="2"/>
+      <c r="S62" s="4">
+        <v>0</v>
+      </c>
+      <c r="X62" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y62" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA62" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD62" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ62" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK62" s="5">
+        <v>924</v>
+      </c>
     </row>
     <row r="63" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
@@ -6240,86 +6316,60 @@
       <c r="B63" s="11">
         <v>1</v>
       </c>
-      <c r="C63" t="s">
-        <v>17</v>
+      <c r="C63" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="D63" t="s">
-        <v>139</v>
-      </c>
-      <c r="E63"/>
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
-      <c r="J63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K63" t="s">
+        <v>204</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K63" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="L63"/>
-      <c r="M63"/>
-      <c r="N63"/>
-      <c r="O63" s="1">
-        <v>0.33</v>
-      </c>
-      <c r="P63" s="1">
-        <v>0.33</v>
-      </c>
-      <c r="Q63">
-        <v>0.95</v>
+      <c r="O63" s="2">
+        <v>1</v>
+      </c>
+      <c r="P63" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="2">
+        <v>0</v>
       </c>
       <c r="R63">
         <v>1</v>
       </c>
-      <c r="S63" s="1">
-        <v>1</v>
-      </c>
-      <c r="T63" s="1"/>
-      <c r="U63" s="1">
-        <v>12</v>
-      </c>
-      <c r="V63" s="1">
-        <v>12</v>
-      </c>
-      <c r="W63" s="1">
-        <v>3.89</v>
-      </c>
-      <c r="X63" s="1">
-        <v>2000</v>
-      </c>
-      <c r="Y63" s="1">
-        <v>3.89</v>
-      </c>
-      <c r="Z63" s="1">
-        <v>100</v>
-      </c>
-      <c r="AA63" s="1">
-        <v>3.89</v>
-      </c>
-      <c r="AB63" s="1">
-        <v>2000</v>
-      </c>
-      <c r="AC63" s="1">
-        <v>12</v>
-      </c>
-      <c r="AD63" s="1">
-        <v>24</v>
-      </c>
-      <c r="AE63">
-        <v>0.05</v>
-      </c>
-      <c r="AF63">
-        <v>0.05</v>
-      </c>
-      <c r="AG63"/>
-      <c r="AH63"/>
-      <c r="AI63"/>
-      <c r="AJ63" s="1">
-        <v>100</v>
-      </c>
-      <c r="AK63"/>
-      <c r="AL63"/>
+      <c r="S63" s="2">
+        <v>0</v>
+      </c>
+      <c r="X63" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y63" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z63" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA63" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB63" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC63" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD63" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ63" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK63" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="64" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
@@ -6328,78 +6378,60 @@
       <c r="B64" s="11">
         <v>1</v>
       </c>
-      <c r="C64" t="s">
-        <v>64</v>
+      <c r="C64" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="D64" t="s">
-        <v>177</v>
-      </c>
-      <c r="E64"/>
-      <c r="F64"/>
-      <c r="G64" t="s">
-        <v>124</v>
-      </c>
-      <c r="H64"/>
-      <c r="I64"/>
-      <c r="J64" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K64" t="s">
+        <v>205</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K64" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="L64"/>
-      <c r="M64"/>
-      <c r="N64"/>
-      <c r="O64">
-        <v>1</v>
-      </c>
-      <c r="P64">
-        <v>1</v>
-      </c>
-      <c r="Q64">
+      <c r="O64" s="2">
+        <v>1</v>
+      </c>
+      <c r="P64" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="2">
         <v>0</v>
       </c>
       <c r="R64">
         <v>1</v>
       </c>
-      <c r="S64">
-        <v>2</v>
-      </c>
-      <c r="T64"/>
-      <c r="U64"/>
-      <c r="V64"/>
-      <c r="W64"/>
-      <c r="X64">
-        <v>0</v>
-      </c>
-      <c r="Y64">
-        <v>0</v>
-      </c>
-      <c r="Z64">
-        <v>0</v>
-      </c>
-      <c r="AA64">
-        <v>0</v>
-      </c>
-      <c r="AB64">
-        <v>0</v>
-      </c>
-      <c r="AC64">
-        <v>0</v>
-      </c>
-      <c r="AD64">
-        <v>0</v>
-      </c>
-      <c r="AE64"/>
-      <c r="AF64"/>
-      <c r="AG64"/>
-      <c r="AH64"/>
-      <c r="AI64"/>
-      <c r="AJ64">
-        <v>0</v>
-      </c>
-      <c r="AK64"/>
-      <c r="AL64"/>
+      <c r="S64" s="2">
+        <v>30</v>
+      </c>
+      <c r="X64" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y64" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK64" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="65" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
@@ -6408,86 +6440,86 @@
       <c r="B65" s="11">
         <v>1</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>54</v>
+      <c r="C65" t="s">
+        <v>17</v>
       </c>
       <c r="D65" t="s">
-        <v>171</v>
-      </c>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
-      <c r="I65" t="s">
-        <v>234</v>
-      </c>
-      <c r="J65" s="8" t="s">
-        <v>46</v>
+        <v>139</v>
+      </c>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
+      <c r="J65" t="s">
+        <v>17</v>
       </c>
       <c r="K65" t="s">
-        <v>223</v>
-      </c>
-      <c r="L65" s="8"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="8"/>
-      <c r="O65" s="8">
-        <v>0.9</v>
-      </c>
-      <c r="P65" s="8">
-        <v>0.9</v>
-      </c>
-      <c r="Q65" s="8">
-        <v>0</v>
+        <v>71</v>
+      </c>
+      <c r="L65"/>
+      <c r="M65"/>
+      <c r="N65"/>
+      <c r="O65" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="P65" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="Q65">
+        <v>0.95</v>
       </c>
       <c r="R65">
         <v>1</v>
       </c>
-      <c r="S65" s="8">
-        <v>2</v>
-      </c>
-      <c r="T65" s="8"/>
-      <c r="U65" s="8">
-        <v>1</v>
-      </c>
-      <c r="V65" s="8">
-        <v>1</v>
-      </c>
-      <c r="W65" s="8">
-        <v>1.94</v>
-      </c>
-      <c r="X65" s="8">
-        <v>15</v>
-      </c>
-      <c r="Y65" s="8">
-        <v>1.94</v>
-      </c>
-      <c r="Z65" s="8">
-        <v>15</v>
-      </c>
-      <c r="AA65" s="8">
-        <v>1.94</v>
-      </c>
-      <c r="AB65" s="8">
-        <v>15</v>
-      </c>
-      <c r="AC65" s="8">
+      <c r="S65" s="1">
+        <v>1</v>
+      </c>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1">
         <v>12</v>
       </c>
-      <c r="AD65" s="8">
+      <c r="V65" s="1">
+        <v>12</v>
+      </c>
+      <c r="W65" s="1">
+        <v>3.89</v>
+      </c>
+      <c r="X65" s="1">
+        <v>2000</v>
+      </c>
+      <c r="Y65" s="1">
+        <v>3.89</v>
+      </c>
+      <c r="Z65" s="1">
+        <v>100</v>
+      </c>
+      <c r="AA65" s="1">
+        <v>3.89</v>
+      </c>
+      <c r="AB65" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AC65" s="1">
+        <v>12</v>
+      </c>
+      <c r="AD65" s="1">
         <v>24</v>
       </c>
-      <c r="AE65" s="8">
+      <c r="AE65">
         <v>0.05</v>
       </c>
-      <c r="AF65" s="8">
+      <c r="AF65">
         <v>0.05</v>
       </c>
-      <c r="AG65" s="8"/>
-      <c r="AH65" s="8"/>
-      <c r="AI65" s="8"/>
-      <c r="AJ65" s="8"/>
-      <c r="AK65" s="8"/>
-      <c r="AL65" s="8"/>
+      <c r="AG65"/>
+      <c r="AH65"/>
+      <c r="AI65"/>
+      <c r="AJ65" s="1">
+        <v>105</v>
+      </c>
+      <c r="AK65"/>
+      <c r="AL65"/>
     </row>
     <row r="66" spans="1:41" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
@@ -6496,88 +6528,78 @@
       <c r="B66" s="11">
         <v>1</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>51</v>
+      <c r="C66" t="s">
+        <v>64</v>
       </c>
       <c r="D66" t="s">
-        <v>169</v>
-      </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" t="s">
-        <v>234</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>49</v>
+        <v>177</v>
+      </c>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66" t="s">
+        <v>124</v>
+      </c>
+      <c r="H66"/>
+      <c r="I66"/>
+      <c r="J66" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="K66" t="s">
         <v>71</v>
       </c>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2"/>
-      <c r="N66" s="2"/>
-      <c r="O66" s="2">
-        <v>0.39</v>
-      </c>
-      <c r="P66" s="2">
-        <v>0.39</v>
-      </c>
-      <c r="Q66" s="2">
-        <v>0.5</v>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66">
+        <v>1</v>
+      </c>
+      <c r="P66">
+        <v>1</v>
+      </c>
+      <c r="Q66">
+        <v>0</v>
       </c>
       <c r="R66">
         <v>1</v>
       </c>
-      <c r="S66" s="2">
-        <v>3.3</v>
-      </c>
-      <c r="T66" s="2"/>
-      <c r="U66" s="2">
-        <v>8</v>
-      </c>
-      <c r="V66" s="2">
-        <v>8</v>
-      </c>
-      <c r="W66" s="2">
-        <v>5</v>
-      </c>
-      <c r="X66" s="2">
-        <v>42</v>
-      </c>
-      <c r="Y66" s="2">
-        <v>5.83</v>
-      </c>
-      <c r="Z66" s="2">
-        <v>57.17</v>
-      </c>
-      <c r="AA66" s="2">
-        <v>2.92</v>
-      </c>
-      <c r="AB66" s="2">
-        <v>31</v>
-      </c>
-      <c r="AC66" s="2">
-        <v>12</v>
-      </c>
-      <c r="AD66" s="2">
-        <v>72</v>
-      </c>
-      <c r="AE66" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AF66" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AG66" s="2"/>
-      <c r="AH66" s="2"/>
-      <c r="AI66" s="2"/>
-      <c r="AJ66" s="2">
-        <v>57.17</v>
-      </c>
-      <c r="AK66" s="2"/>
-      <c r="AL66" s="2"/>
+      <c r="S66">
+        <v>2</v>
+      </c>
+      <c r="T66"/>
+      <c r="U66"/>
+      <c r="V66"/>
+      <c r="W66"/>
+      <c r="X66">
+        <v>0</v>
+      </c>
+      <c r="Y66">
+        <v>0</v>
+      </c>
+      <c r="Z66">
+        <v>0</v>
+      </c>
+      <c r="AA66">
+        <v>0</v>
+      </c>
+      <c r="AB66">
+        <v>0</v>
+      </c>
+      <c r="AC66">
+        <v>0</v>
+      </c>
+      <c r="AD66">
+        <v>0</v>
+      </c>
+      <c r="AE66"/>
+      <c r="AF66"/>
+      <c r="AG66"/>
+      <c r="AH66"/>
+      <c r="AI66"/>
+      <c r="AJ66">
+        <v>0</v>
+      </c>
+      <c r="AK66"/>
+      <c r="AL66"/>
     </row>
     <row r="67" spans="1:41" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
@@ -6586,88 +6608,86 @@
       <c r="B67" s="11">
         <v>1</v>
       </c>
-      <c r="C67" t="s">
-        <v>52</v>
+      <c r="C67" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="D67" t="s">
-        <v>170</v>
-      </c>
-      <c r="E67"/>
-      <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67"/>
+        <v>171</v>
+      </c>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
       <c r="I67" t="s">
         <v>234</v>
       </c>
-      <c r="J67" t="s">
-        <v>49</v>
+      <c r="J67" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="K67" t="s">
-        <v>71</v>
-      </c>
-      <c r="L67"/>
-      <c r="M67"/>
-      <c r="N67"/>
-      <c r="O67">
-        <v>0.39</v>
-      </c>
-      <c r="P67">
-        <v>0.39</v>
-      </c>
-      <c r="Q67">
-        <v>0.5</v>
+        <v>223</v>
+      </c>
+      <c r="L67" s="8"/>
+      <c r="M67" s="8"/>
+      <c r="N67" s="8"/>
+      <c r="O67" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P67" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="Q67" s="8">
+        <v>0</v>
       </c>
       <c r="R67">
         <v>1</v>
       </c>
-      <c r="S67">
-        <v>3.3</v>
-      </c>
-      <c r="T67"/>
-      <c r="U67">
-        <v>8</v>
-      </c>
-      <c r="V67">
-        <v>8</v>
-      </c>
-      <c r="W67">
-        <v>5</v>
-      </c>
-      <c r="X67">
-        <v>42</v>
-      </c>
-      <c r="Y67">
-        <v>5.83</v>
-      </c>
-      <c r="Z67">
-        <v>57.17</v>
-      </c>
-      <c r="AA67">
-        <v>2.92</v>
-      </c>
-      <c r="AB67">
-        <v>31</v>
-      </c>
-      <c r="AC67">
+      <c r="S67" s="8">
+        <v>2</v>
+      </c>
+      <c r="T67" s="8"/>
+      <c r="U67" s="8">
+        <v>1</v>
+      </c>
+      <c r="V67" s="8">
+        <v>1</v>
+      </c>
+      <c r="W67" s="8">
+        <v>1.94</v>
+      </c>
+      <c r="X67" s="8">
+        <v>15</v>
+      </c>
+      <c r="Y67" s="8">
+        <v>1.94</v>
+      </c>
+      <c r="Z67" s="8">
+        <v>15</v>
+      </c>
+      <c r="AA67" s="8">
+        <v>1.94</v>
+      </c>
+      <c r="AB67" s="8">
+        <v>15</v>
+      </c>
+      <c r="AC67" s="8">
         <v>12</v>
       </c>
-      <c r="AD67">
-        <v>72</v>
-      </c>
-      <c r="AE67">
-        <v>0.08</v>
-      </c>
-      <c r="AF67">
-        <v>0.08</v>
-      </c>
-      <c r="AG67"/>
-      <c r="AH67"/>
-      <c r="AI67"/>
-      <c r="AJ67">
-        <v>57.17</v>
-      </c>
-      <c r="AK67"/>
-      <c r="AL67"/>
+      <c r="AD67" s="8">
+        <v>24</v>
+      </c>
+      <c r="AE67" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="AF67" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="AG67" s="8"/>
+      <c r="AH67" s="8"/>
+      <c r="AI67" s="8"/>
+      <c r="AJ67" s="8"/>
+      <c r="AK67" s="8"/>
+      <c r="AL67" s="8"/>
     </row>
     <row r="68" spans="1:41" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
@@ -6677,10 +6697,10 @@
         <v>1</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D68" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -6699,10 +6719,10 @@
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.39</v>
       </c>
       <c r="P68" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.39</v>
       </c>
       <c r="Q68" s="2">
         <v>0.5</v>
@@ -6715,28 +6735,28 @@
       </c>
       <c r="T68" s="2"/>
       <c r="U68" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="V68" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="W68" s="2">
         <v>5</v>
       </c>
       <c r="X68" s="2">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="Y68" s="2">
         <v>5.83</v>
       </c>
       <c r="Z68" s="2">
-        <v>88</v>
+        <v>57.17</v>
       </c>
       <c r="AA68" s="2">
         <v>2.92</v>
       </c>
       <c r="AB68" s="2">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="AC68" s="2">
         <v>12</v>
@@ -6754,7 +6774,7 @@
       <c r="AH68" s="2"/>
       <c r="AI68" s="2"/>
       <c r="AJ68" s="2">
-        <v>88</v>
+        <v>57.17</v>
       </c>
       <c r="AK68" s="2"/>
       <c r="AL68" s="2"/>
@@ -6767,20 +6787,20 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D69" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E69"/>
       <c r="F69"/>
-      <c r="G69" t="s">
-        <v>123</v>
-      </c>
+      <c r="G69"/>
       <c r="H69"/>
-      <c r="I69"/>
-      <c r="J69" s="8" t="s">
-        <v>18</v>
+      <c r="I69" t="s">
+        <v>234</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="K69" t="s">
         <v>71</v>
@@ -6789,55 +6809,65 @@
       <c r="M69"/>
       <c r="N69"/>
       <c r="O69">
-        <v>1</v>
+        <v>0.39</v>
       </c>
       <c r="P69">
-        <v>1</v>
+        <v>0.39</v>
       </c>
       <c r="Q69">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R69">
         <v>1</v>
       </c>
       <c r="S69">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="T69"/>
-      <c r="U69"/>
-      <c r="V69"/>
-      <c r="W69"/>
+      <c r="U69">
+        <v>8</v>
+      </c>
+      <c r="V69">
+        <v>8</v>
+      </c>
+      <c r="W69">
+        <v>5</v>
+      </c>
       <c r="X69">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="Y69">
-        <v>0</v>
+        <v>5.83</v>
       </c>
       <c r="Z69">
-        <v>0</v>
+        <v>57.17</v>
       </c>
       <c r="AA69">
-        <v>0</v>
+        <v>2.92</v>
       </c>
       <c r="AB69">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AC69">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AD69">
-        <v>0</v>
-      </c>
-      <c r="AE69"/>
-      <c r="AF69"/>
+        <v>72</v>
+      </c>
+      <c r="AE69">
+        <v>0.08</v>
+      </c>
+      <c r="AF69">
+        <v>0.08</v>
+      </c>
       <c r="AG69"/>
       <c r="AH69"/>
       <c r="AI69"/>
       <c r="AJ69">
-        <v>0</v>
+        <v>57.17</v>
       </c>
       <c r="AK69"/>
-      <c r="AL69" s="2"/>
+      <c r="AL69"/>
     </row>
     <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
@@ -6846,92 +6876,87 @@
       <c r="B70" s="11">
         <v>1</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>241</v>
+      <c r="C70" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D70" t="s">
-        <v>243</v>
-      </c>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
+        <v>168</v>
+      </c>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
       <c r="I70" t="s">
         <v>234</v>
       </c>
-      <c r="J70" s="6" t="s">
-        <v>19</v>
+      <c r="J70" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="K70" t="s">
         <v>71</v>
       </c>
-      <c r="L70" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="M70" s="6"/>
-      <c r="N70" s="6"/>
-      <c r="O70" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="P70" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="Q70" s="4">
-        <v>0.4</v>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="P70" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q70" s="2">
+        <v>0.5</v>
       </c>
       <c r="R70">
         <v>1</v>
       </c>
-      <c r="S70" s="4">
-        <v>2</v>
-      </c>
-      <c r="T70" s="4"/>
-      <c r="U70" s="4">
-        <v>3</v>
-      </c>
-      <c r="V70" s="4">
-        <v>3</v>
-      </c>
-      <c r="W70" s="4">
-        <v>1.94</v>
-      </c>
-      <c r="X70" s="4">
-        <v>70</v>
-      </c>
-      <c r="Y70" s="4">
-        <v>1.94</v>
-      </c>
-      <c r="Z70" s="4">
-        <v>150</v>
-      </c>
-      <c r="AA70" s="4">
-        <v>1.94</v>
-      </c>
-      <c r="AB70" s="4">
-        <v>40</v>
-      </c>
-      <c r="AC70" s="4">
+      <c r="S70" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="T70" s="2"/>
+      <c r="U70" s="2">
+        <v>11</v>
+      </c>
+      <c r="V70" s="2">
+        <v>11</v>
+      </c>
+      <c r="W70" s="2">
+        <v>5</v>
+      </c>
+      <c r="X70" s="2">
+        <v>60</v>
+      </c>
+      <c r="Y70" s="2">
+        <v>5.83</v>
+      </c>
+      <c r="Z70" s="2">
+        <v>88</v>
+      </c>
+      <c r="AA70" s="2">
+        <v>2.92</v>
+      </c>
+      <c r="AB70" s="2">
+        <v>46</v>
+      </c>
+      <c r="AC70" s="2">
         <v>12</v>
       </c>
-      <c r="AD70" s="4">
-        <v>24</v>
-      </c>
-      <c r="AE70" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="AF70" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="AG70" s="4"/>
-      <c r="AH70" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="AI70" s="4">
-        <v>-0.16666666666666699</v>
-      </c>
-      <c r="AJ70" s="4">
-        <v>150</v>
-      </c>
+      <c r="AD70" s="2">
+        <v>72</v>
+      </c>
+      <c r="AE70" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="AF70" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="AG70" s="2"/>
+      <c r="AH70" s="2"/>
+      <c r="AI70" s="2"/>
+      <c r="AJ70" s="2">
+        <v>88</v>
+      </c>
+      <c r="AK70" s="2"/>
       <c r="AL70" s="2"/>
       <c r="AM70" s="4"/>
       <c r="AN70" s="4"/>
@@ -6944,90 +6969,61 @@
       <c r="B71" s="11">
         <v>1</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>242</v>
+      <c r="C71" t="s">
+        <v>62</v>
       </c>
       <c r="D71" t="s">
-        <v>244</v>
-      </c>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
-      <c r="J71" s="6" t="s">
-        <v>56</v>
+        <v>176</v>
+      </c>
+      <c r="G71" t="s">
+        <v>123</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="K71" t="s">
         <v>71</v>
       </c>
-      <c r="L71" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="P71" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="Q71" s="4">
-        <v>0.4</v>
+      <c r="O71">
+        <v>1</v>
+      </c>
+      <c r="P71">
+        <v>1</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
       </c>
       <c r="R71">
         <v>1</v>
       </c>
-      <c r="S71" s="4">
+      <c r="S71">
         <v>2</v>
       </c>
-      <c r="T71" s="4"/>
-      <c r="U71" s="4">
-        <v>3</v>
-      </c>
-      <c r="V71" s="4">
-        <v>3</v>
-      </c>
-      <c r="W71" s="4">
-        <v>1.94</v>
-      </c>
-      <c r="X71" s="4">
-        <v>70</v>
-      </c>
-      <c r="Y71" s="4">
-        <v>1.94</v>
-      </c>
-      <c r="Z71" s="4">
-        <v>150</v>
-      </c>
-      <c r="AA71" s="4">
-        <v>1.94</v>
-      </c>
-      <c r="AB71" s="4">
-        <v>40</v>
-      </c>
-      <c r="AC71" s="4">
-        <v>12</v>
-      </c>
-      <c r="AD71" s="4">
-        <v>24</v>
-      </c>
-      <c r="AE71" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="AF71" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="AG71" s="4"/>
-      <c r="AH71" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="AI71" s="4">
-        <v>-0.16666666666666699</v>
-      </c>
-      <c r="AJ71" s="4">
-        <v>90</v>
-      </c>
+      <c r="X71">
+        <v>0</v>
+      </c>
+      <c r="Y71">
+        <v>0</v>
+      </c>
+      <c r="Z71">
+        <v>0</v>
+      </c>
+      <c r="AA71">
+        <v>0</v>
+      </c>
+      <c r="AB71">
+        <v>0</v>
+      </c>
+      <c r="AC71">
+        <v>0</v>
+      </c>
+      <c r="AD71">
+        <v>0</v>
+      </c>
+      <c r="AJ71">
+        <v>0</v>
+      </c>
+      <c r="AL71" s="2"/>
     </row>
     <row r="72" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">

</xml_diff>